<commit_message>
Update Zoster schedule: varicella (178) has been added as a contra-indication
</commit_message>
<xml_diff>
--- a/schedules/Zoster.xlsx
+++ b/schedules/Zoster.xlsx
@@ -5,25 +5,25 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\forecast\forecaster2012\schedules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gbkerr\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="283"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="6192" tabRatio="283"/>
   </bookViews>
   <sheets>
     <sheet name="Schedules" sheetId="1" r:id="rId1"/>
     <sheet name="XML" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Schedules!$A$1:$K$47</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Schedules!$A$1:$K$49</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="60">
   <si>
     <t>Forecast Series Name</t>
   </si>
@@ -199,7 +199,10 @@
     <t>Influenza LAIV4 Nasal</t>
   </si>
   <si>
-    <t>160, 161, 158, 162, 171, 175, 180, 2020, 1990, 148, 1690, 1700, 210, 203</t>
+    <t>varicella</t>
+  </si>
+  <si>
+    <t>160, 161, 158, 162, 171, 175, 178, 180, 2020, 1990, 148, 1690, 1700, 210, 203</t>
   </si>
 </sst>
 </file>
@@ -447,7 +450,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -537,6 +540,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -971,34 +977,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J46"/>
+  <dimension ref="B1:J48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.5703125" style="1" customWidth="1"/>
-    <col min="2" max="3" width="14.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" style="1" customWidth="1"/>
-    <col min="6" max="7" width="12.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="1.5546875" style="1" customWidth="1"/>
+    <col min="2" max="3" width="14.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="1" customWidth="1"/>
+    <col min="6" max="7" width="12.44140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="18" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="17.140625" style="1" customWidth="1"/>
-    <col min="13" max="16" width="11.5703125" style="1"/>
-    <col min="17" max="17" width="6.28515625" style="1" customWidth="1"/>
-    <col min="18" max="22" width="11.5703125" style="1"/>
-    <col min="23" max="23" width="6.28515625" style="1" customWidth="1"/>
-    <col min="24" max="24" width="3.28515625" style="1" customWidth="1"/>
-    <col min="25" max="16384" width="11.5703125" style="1"/>
+    <col min="9" max="9" width="11.109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="17.109375" style="1" customWidth="1"/>
+    <col min="13" max="16" width="11.5546875" style="1"/>
+    <col min="17" max="17" width="6.33203125" style="1" customWidth="1"/>
+    <col min="18" max="22" width="11.5546875" style="1"/>
+    <col min="23" max="23" width="6.33203125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="3.33203125" style="1" customWidth="1"/>
+    <col min="25" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1014,7 +1020,7 @@
       <c r="I2" s="26"/>
       <c r="J2" s="26"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
@@ -1034,7 +1040,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
         <v>6</v>
       </c>
@@ -1052,7 +1058,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F5" s="10" t="s">
         <v>47</v>
       </c>
@@ -1063,12 +1069,12 @@
         <v>2110</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:10" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="33" t="s">
         <v>52</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D6" s="28"/>
       <c r="F6" s="10"/>
@@ -1077,7 +1083,7 @@
       <c r="I6" s="11"/>
       <c r="J6" s="9"/>
     </row>
-    <row r="7" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="34"/>
       <c r="C7" s="29"/>
       <c r="D7" s="30"/>
@@ -1087,7 +1093,7 @@
       <c r="I7" s="11"/>
       <c r="J7" s="9"/>
     </row>
-    <row r="8" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="35"/>
       <c r="C8" s="31"/>
       <c r="D8" s="32"/>
@@ -1097,11 +1103,11 @@
       <c r="I8" s="11"/>
       <c r="J8" s="9"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F10" s="26" t="s">
         <v>9</v>
       </c>
@@ -1110,7 +1116,7 @@
       <c r="I10" s="26"/>
       <c r="J10" s="26"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F11" s="7" t="s">
         <v>3</v>
       </c>
@@ -1123,7 +1129,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F12" s="10" t="s">
         <v>10</v>
       </c>
@@ -1134,7 +1140,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F13" s="10" t="s">
         <v>11</v>
       </c>
@@ -1145,7 +1151,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F14" s="10" t="s">
         <v>12</v>
       </c>
@@ -1156,7 +1162,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F15" s="10" t="s">
         <v>13</v>
       </c>
@@ -1167,7 +1173,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F16" s="10" t="s">
         <v>14</v>
       </c>
@@ -1178,7 +1184,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F17" s="10" t="s">
         <v>15</v>
       </c>
@@ -1189,297 +1195,308 @@
         <v>175</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F18" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="G18" s="15"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="9">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F19" s="10" t="s">
         <v>16</v>
-      </c>
-      <c r="G18" s="15"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="9">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="F19" s="10" t="s">
-        <v>57</v>
       </c>
       <c r="G19" s="15"/>
       <c r="H19" s="12"/>
       <c r="I19" s="10"/>
       <c r="J19" s="9">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F20" s="10" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="G20" s="15"/>
       <c r="H20" s="12"/>
       <c r="I20" s="10"/>
       <c r="J20" s="9">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F21" s="10" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="G21" s="15"/>
       <c r="H21" s="12"/>
       <c r="I21" s="10"/>
       <c r="J21" s="9">
-        <v>1990</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F22" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G22" s="15"/>
       <c r="H22" s="12"/>
       <c r="I22" s="10"/>
       <c r="J22" s="9">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+        <v>1990</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F23" s="10" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="G23" s="15"/>
       <c r="H23" s="12"/>
       <c r="I23" s="10"/>
       <c r="J23" s="9">
-        <v>1690</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F24" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G24" s="15"/>
       <c r="H24" s="12"/>
       <c r="I24" s="10"/>
       <c r="J24" s="9">
-        <v>1700</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F25" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G25" s="15"/>
       <c r="H25" s="12"/>
       <c r="I25" s="10"/>
       <c r="J25" s="9">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F26" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G26" s="15"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="9">
         <v>210</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B28" s="5" t="s">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C30" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D30" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E28" s="16" t="s">
+      <c r="E30" s="16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B29" s="17" t="s">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B31" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="17">
+      <c r="C31" s="17">
         <v>1</v>
       </c>
-      <c r="D29" s="17" t="s">
+      <c r="D31" s="17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B30" s="26" t="s">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B32" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B31" s="18"/>
-      <c r="C31" s="6" t="s">
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="18"/>
+      <c r="C33" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D33" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E31" s="6" t="s">
+      <c r="E33" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B32" s="19" t="s">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C34" s="9" t="s">
         <v>56</v>
-      </c>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B33" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B34" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>50</v>
       </c>
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>54</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C35" s="9"/>
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B37" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="C37" s="21"/>
-      <c r="D37" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B38" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="C38" s="21"/>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>51</v>
+      </c>
       <c r="D38" s="9"/>
       <c r="E38" s="9"/>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B39" s="26" t="s">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C39" s="21"/>
+      <c r="D39" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C40" s="21"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B40" s="6" t="s">
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C42" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="D42" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E40" s="6" t="s">
+      <c r="E42" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F40" s="6" t="s">
+      <c r="F42" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B41" s="9" t="s">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B43" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C41" s="9" t="s">
+      <c r="C43" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B42" s="26" t="s">
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B44" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="C42" s="26"/>
-      <c r="D42" s="26"/>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B43" s="6" t="s">
+      <c r="C44" s="26"/>
+      <c r="D44" s="26"/>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B45" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C45" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="D45" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E43" s="6" t="s">
+      <c r="E45" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B44" s="9" t="s">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B46" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C44" s="9" t="s">
+      <c r="C46" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D44" s="9"/>
-      <c r="E44" s="22"/>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B45" s="19" t="s">
+      <c r="D46" s="9"/>
+      <c r="E46" s="22"/>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B47" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C45" s="9">
+      <c r="C47" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B46" s="19" t="s">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B48" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="C46" s="9">
+      <c r="C48" s="9">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="7">
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B44:D44"/>
     <mergeCell ref="F2:J2"/>
     <mergeCell ref="F10:J10"/>
-    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B32:E32"/>
     <mergeCell ref="C6:D8"/>
     <mergeCell ref="B6:B8"/>
   </mergeCells>
@@ -1491,7 +1508,7 @@
     <oddFooter>&amp;CPrepared by  Nathan Bunker &amp;D&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="26" max="16383" man="1"/>
+    <brk id="28" max="16383" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
@@ -1501,105 +1518,105 @@
   <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A16"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="106.28515625" customWidth="1"/>
+    <col min="1" max="1" width="106.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="str">
         <f>"&lt;forecast seriesName="&amp;CHAR(34)&amp;Schedules!D2&amp;CHAR(34)&amp;"&gt;"</f>
         <v>&lt;forecast seriesName="Zoster"&gt;</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B4&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C4&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="Single" vaccineIds="2010, 2110"/&gt;</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B6&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C6&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">  &lt;vaccine vaccineName="Live" vaccineIds="160, 161, 158, 162, 171, 175, 180, 2020, 1990, 148, 1690, 1700, 210, 203"/&gt;</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+        <v xml:space="preserve">  &lt;vaccine vaccineName="Live" vaccineIds="160, 161, 158, 162, 171, 175, 178, 180, 2020, 1990, 148, 1690, 1700, 210, 203"/&gt;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="str">
-        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B29&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C29&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D29&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E28&amp;CHAR(34)&amp;"&gt;"</f>
+        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B31&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C31&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D31&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E30&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="P1" dose="1" indication="BIRTH" label="1 year"&gt;</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="str">
-        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C46&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C45&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C48&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C47&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="1"/&gt;</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="str">
-        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C32&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D32&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E32&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C34&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D34&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E34&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="50 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="str">
-        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C33&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D33&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E33&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C35&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D35&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E35&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="str">
-        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C34&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D34&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E34&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C36&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D36&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E36&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="60 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="str">
-        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C35&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D35&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E35&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C37&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D37&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E37&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="61 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="str">
-        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C36&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D36&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E36&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C38&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D38&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E38&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="120 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="str">
-        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D37&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E37&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D39&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E39&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="24" t="str">
-        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D38&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D40&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="str">
-        <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B41&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C41&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D41&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E41&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!F41&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B43&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C43&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D43&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E43&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!F43&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;contraindicate vaccineName="Live" afterInterval="4 weeks" age="" reason="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B44&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C44&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D44&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E44&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B46&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C46&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D46&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E46&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Single" schedule="COMPLETE" age="" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="str">
         <f>"&lt;/forecast&gt;"</f>
         <v>&lt;/forecast&gt;</v>

</xml_diff>

<commit_message>
Add updated Zoster schedule
Note: the changes were already committed. I simply made a trivial change so they could be recommitted.
</commit_message>
<xml_diff>
--- a/schedules/Zoster.xlsx
+++ b/schedules/Zoster.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TCH\TCHWorkspaces\iris006-ws\fv\schedules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TCHWorkspaceJava6\fv\schedules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1185" yWindow="0" windowWidth="20445" windowHeight="13680" tabRatio="283" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2490" yWindow="0" windowWidth="20445" windowHeight="13680" tabRatio="283"/>
   </bookViews>
   <sheets>
     <sheet name="Schedules" sheetId="1" r:id="rId1"/>
@@ -192,7 +192,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
   </numFmts>
@@ -483,20 +483,20 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -933,11 +933,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J90"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -963,13 +963,13 @@
       <c r="D2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="37" t="s">
+      <c r="F2" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
@@ -1042,8 +1042,8 @@
     </row>
     <row r="7" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="17"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
       <c r="H7" s="18"/>
       <c r="I7" s="18"/>
     </row>
@@ -1073,12 +1073,12 @@
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B19" s="39" t="s">
+      <c r="B19" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="41"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="39"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" s="22"/>
@@ -1163,11 +1163,11 @@
       <c r="E27" s="14"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B28" s="37" t="s">
+      <c r="B28" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B29" s="7" t="s">
@@ -1240,12 +1240,12 @@
       </c>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B38" s="39" t="s">
+      <c r="B38" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="C38" s="40"/>
-      <c r="D38" s="40"/>
-      <c r="E38" s="41"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="39"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B39" s="22"/>
@@ -1331,11 +1331,11 @@
       <c r="E46" s="14"/>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B47" s="37" t="s">
+      <c r="B47" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="C47" s="37"/>
-      <c r="D47" s="37"/>
+      <c r="C47" s="40"/>
+      <c r="D47" s="40"/>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B48" s="7" t="s">
@@ -1414,12 +1414,12 @@
       </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B57" s="39" t="s">
+      <c r="B57" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="C57" s="40"/>
-      <c r="D57" s="40"/>
-      <c r="E57" s="41"/>
+      <c r="C57" s="38"/>
+      <c r="D57" s="38"/>
+      <c r="E57" s="39"/>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B58" s="22"/>
@@ -1500,11 +1500,11 @@
       <c r="E65" s="14"/>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B66" s="37" t="s">
+      <c r="B66" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="C66" s="37"/>
-      <c r="D66" s="37"/>
+      <c r="C66" s="40"/>
+      <c r="D66" s="40"/>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B67" s="7" t="s">
@@ -1577,12 +1577,12 @@
       </c>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B76" s="39" t="s">
+      <c r="B76" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="C76" s="40"/>
-      <c r="D76" s="40"/>
-      <c r="E76" s="41"/>
+      <c r="C76" s="38"/>
+      <c r="D76" s="38"/>
+      <c r="E76" s="39"/>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B77" s="22"/>
@@ -1663,11 +1663,11 @@
       <c r="E84" s="14"/>
     </row>
     <row r="85" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B85" s="37" t="s">
+      <c r="B85" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="C85" s="37"/>
-      <c r="D85" s="37"/>
+      <c r="C85" s="40"/>
+      <c r="D85" s="40"/>
     </row>
     <row r="86" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B86" s="7" t="s">
@@ -1722,16 +1722,16 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="10">
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B38:E38"/>
     <mergeCell ref="B57:E57"/>
     <mergeCell ref="B66:D66"/>
     <mergeCell ref="B76:E76"/>
     <mergeCell ref="B85:D85"/>
     <mergeCell ref="B47:D47"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B38:E38"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1748,7 +1748,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A52"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Release 4.1.1 with latest Zoster schedule changes
</commit_message>
<xml_diff>
--- a/schedules/Zoster.xlsx
+++ b/schedules/Zoster.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TCHWorkspaceJava6\fv\schedules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Forecaster Schedule Updates\Zostre Updates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2565" yWindow="0" windowWidth="18705" windowHeight="11535" tabRatio="365"/>
+    <workbookView xWindow="3555" yWindow="0" windowWidth="16140" windowHeight="11025" tabRatio="283"/>
   </bookViews>
   <sheets>
     <sheet name="Schedules" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,12 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Schedules!$A$1:$K$144</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="57">
   <si>
     <t>Forecast Series Name</t>
   </si>
@@ -134,9 +134,6 @@
   </si>
   <si>
     <t>7 months</t>
-  </si>
-  <si>
-    <t>4 weeks 4 days</t>
   </si>
   <si>
     <t>P1a</t>
@@ -532,7 +529,6 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -575,9 +571,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -642,12 +635,16 @@
     <xf numFmtId="0" fontId="3" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="21" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -660,17 +657,17 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="20" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -746,10 +743,10 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
     <mruColors>
+      <color rgb="FFCCFFCC"/>
+      <color rgb="FFFFCCFF"/>
       <color rgb="FFFFCCCC"/>
       <color rgb="FFCCCCFF"/>
-      <color rgb="FFCCFFCC"/>
-      <color rgb="FFFFCCFF"/>
       <color rgb="FF993300"/>
       <color rgb="FFFFFFCC"/>
       <color rgb="FF33CCCC"/>
@@ -772,39 +769,39 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>248708</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>100542</xdr:rowOff>
+      <xdr:colOff>52918</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>42334</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>359833</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>188355</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>52451</xdr:rowOff>
+      <xdr:rowOff>27430</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="354541" y="2111375"/>
-          <a:ext cx="8143875" cy="6301909"/>
+          <a:off x="158751" y="2211917"/>
+          <a:ext cx="9120687" cy="6176346"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1166,37 +1163,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O143"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="1.5703125" style="13" customWidth="1"/>
-    <col min="2" max="3" width="14.28515625" style="13" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="13" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" style="13" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" style="13" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" style="13" customWidth="1"/>
-    <col min="8" max="8" width="18" style="13" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="13" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" style="13" customWidth="1"/>
-    <col min="11" max="11" width="4.7109375" style="13" customWidth="1"/>
-    <col min="12" max="12" width="17.140625" style="13" customWidth="1"/>
-    <col min="13" max="16" width="11.5703125" style="13"/>
-    <col min="17" max="17" width="6.28515625" style="13" customWidth="1"/>
-    <col min="18" max="22" width="11.5703125" style="13"/>
-    <col min="23" max="23" width="6.28515625" style="13" customWidth="1"/>
-    <col min="24" max="24" width="3.28515625" style="13" customWidth="1"/>
-    <col min="25" max="16384" width="11.5703125" style="13"/>
+    <col min="1" max="1" width="1.5703125" style="12" customWidth="1"/>
+    <col min="2" max="3" width="14.28515625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" style="12" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" style="12" customWidth="1"/>
+    <col min="8" max="8" width="18" style="12" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" style="12" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" style="12" customWidth="1"/>
+    <col min="11" max="11" width="4.7109375" style="12" customWidth="1"/>
+    <col min="12" max="12" width="17.140625" style="12" customWidth="1"/>
+    <col min="13" max="16" width="11.5703125" style="12"/>
+    <col min="17" max="17" width="6.28515625" style="12" customWidth="1"/>
+    <col min="18" max="22" width="11.5703125" style="12"/>
+    <col min="23" max="23" width="6.28515625" style="12" customWidth="1"/>
+    <col min="24" max="24" width="3.28515625" style="12" customWidth="1"/>
+    <col min="25" max="16384" width="11.5703125" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="16" t="s">
-        <v>57</v>
+      <c r="C2" s="14"/>
+      <c r="D2" s="15" t="s">
+        <v>56</v>
       </c>
       <c r="F2" s="62" t="s">
         <v>1</v>
@@ -1207,413 +1204,413 @@
       <c r="J2" s="62"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="F3" s="18" t="s">
+      <c r="D3" s="18"/>
+      <c r="F3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="19"/>
-      <c r="H3" s="18" t="s">
+      <c r="G3" s="18"/>
+      <c r="H3" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="19"/>
-      <c r="J3" s="17" t="s">
+      <c r="I3" s="18"/>
+      <c r="J3" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="20">
         <v>2110</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="F4" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="G4" s="24"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="25">
+      <c r="D4" s="21"/>
+      <c r="F4" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="23"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="24">
         <v>2110</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B5" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="27">
+      <c r="B5" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="26">
         <v>237</v>
       </c>
-      <c r="D5" s="28"/>
-      <c r="F5" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="G5" s="24"/>
-      <c r="H5" s="23" t="s">
+      <c r="D5" s="27"/>
+      <c r="F5" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="23"/>
+      <c r="H5" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="22"/>
-      <c r="J5" s="25">
+      <c r="I5" s="21"/>
+      <c r="J5" s="24">
         <v>237</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="F6" s="23"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="25"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="24"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="F7" s="23"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="25"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="24"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B9" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" s="66">
+      <c r="B9" s="59" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="68">
         <v>178</v>
       </c>
-      <c r="D9" s="67"/>
-      <c r="F9" s="68" t="s">
-        <v>50</v>
-      </c>
-      <c r="G9" s="69"/>
-      <c r="H9" s="69"/>
-      <c r="I9" s="69"/>
-      <c r="J9" s="69"/>
+      <c r="D9" s="69"/>
+      <c r="F9" s="66" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" s="67"/>
+      <c r="H9" s="67"/>
+      <c r="I9" s="67"/>
+      <c r="J9" s="67"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B10" s="31"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="F10" s="18" t="s">
+      <c r="B10" s="29"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="F10" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="G10" s="33"/>
-      <c r="H10" s="18" t="s">
+      <c r="G10" s="31"/>
+      <c r="H10" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="I10" s="34"/>
-      <c r="J10" s="17" t="s">
+      <c r="I10" s="32"/>
+      <c r="J10" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B11" s="31"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="F11" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="G11" s="35"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="25">
+      <c r="B11" s="29"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="F11" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="33"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="24">
         <v>178</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="F12" s="37"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="38"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="36"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="F13" s="37"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="38"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="36"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="F14" s="37"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="38"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="36"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="F15" s="37"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="38"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="36"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="F16" s="37"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="38"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="36"/>
     </row>
     <row r="17" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F17" s="37"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="38"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="36"/>
     </row>
     <row r="18" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F18" s="37"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="38"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="36"/>
     </row>
     <row r="19" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F19" s="37"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="38"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="36"/>
     </row>
     <row r="20" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F20" s="37"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="38"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="36"/>
     </row>
     <row r="21" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F21" s="37"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="37"/>
-      <c r="I21" s="38"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="36"/>
     </row>
     <row r="22" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F22" s="37"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="37"/>
-      <c r="I22" s="38"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="36"/>
     </row>
     <row r="23" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F23" s="37"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="38"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="35"/>
+      <c r="I23" s="36"/>
     </row>
     <row r="24" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F24" s="37"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="37"/>
-      <c r="I24" s="38"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="35"/>
+      <c r="I24" s="36"/>
     </row>
     <row r="25" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F25" s="37"/>
-      <c r="G25" s="38"/>
-      <c r="H25" s="37"/>
-      <c r="I25" s="38"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="35"/>
+      <c r="I25" s="36"/>
     </row>
     <row r="26" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F26" s="37"/>
-      <c r="G26" s="38"/>
-      <c r="H26" s="37"/>
-      <c r="I26" s="38"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="35"/>
+      <c r="I26" s="36"/>
     </row>
     <row r="27" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F27" s="37"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="38"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="35"/>
+      <c r="I27" s="36"/>
     </row>
     <row r="28" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F28" s="37"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="38"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="35"/>
+      <c r="I28" s="36"/>
     </row>
     <row r="29" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F29" s="37"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="38"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="36"/>
+      <c r="H29" s="35"/>
+      <c r="I29" s="36"/>
     </row>
     <row r="30" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F30" s="37"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="37"/>
-      <c r="I30" s="38"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="35"/>
+      <c r="I30" s="36"/>
     </row>
     <row r="31" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F31" s="37"/>
-      <c r="G31" s="38"/>
-      <c r="H31" s="37"/>
-      <c r="I31" s="38"/>
+      <c r="F31" s="35"/>
+      <c r="G31" s="36"/>
+      <c r="H31" s="35"/>
+      <c r="I31" s="36"/>
     </row>
     <row r="32" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F32" s="37"/>
-      <c r="G32" s="38"/>
-      <c r="H32" s="37"/>
-      <c r="I32" s="38"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="36"/>
+      <c r="H32" s="35"/>
+      <c r="I32" s="36"/>
     </row>
     <row r="33" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F33" s="37"/>
-      <c r="G33" s="38"/>
-      <c r="H33" s="37"/>
-      <c r="I33" s="38"/>
+      <c r="F33" s="35"/>
+      <c r="G33" s="36"/>
+      <c r="H33" s="35"/>
+      <c r="I33" s="36"/>
     </row>
     <row r="34" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F34" s="37"/>
-      <c r="G34" s="38"/>
-      <c r="H34" s="37"/>
-      <c r="I34" s="38"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="36"/>
+      <c r="H34" s="35"/>
+      <c r="I34" s="36"/>
     </row>
     <row r="35" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F35" s="37"/>
-      <c r="G35" s="38"/>
-      <c r="H35" s="37"/>
-      <c r="I35" s="38"/>
+      <c r="F35" s="35"/>
+      <c r="G35" s="36"/>
+      <c r="H35" s="35"/>
+      <c r="I35" s="36"/>
     </row>
     <row r="36" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F36" s="37"/>
-      <c r="G36" s="38"/>
-      <c r="H36" s="37"/>
-      <c r="I36" s="38"/>
+      <c r="F36" s="35"/>
+      <c r="G36" s="36"/>
+      <c r="H36" s="35"/>
+      <c r="I36" s="36"/>
     </row>
     <row r="37" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F37" s="37"/>
-      <c r="G37" s="38"/>
-      <c r="H37" s="37"/>
-      <c r="I37" s="38"/>
+      <c r="F37" s="35"/>
+      <c r="G37" s="36"/>
+      <c r="H37" s="35"/>
+      <c r="I37" s="36"/>
     </row>
     <row r="38" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F38" s="37"/>
-      <c r="G38" s="38"/>
-      <c r="H38" s="37"/>
-      <c r="I38" s="38"/>
+      <c r="F38" s="35"/>
+      <c r="G38" s="36"/>
+      <c r="H38" s="35"/>
+      <c r="I38" s="36"/>
     </row>
     <row r="39" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F39" s="37"/>
-      <c r="G39" s="38"/>
-      <c r="H39" s="37"/>
-      <c r="I39" s="38"/>
+      <c r="F39" s="35"/>
+      <c r="G39" s="36"/>
+      <c r="H39" s="35"/>
+      <c r="I39" s="36"/>
     </row>
     <row r="40" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F40" s="37"/>
-      <c r="G40" s="38"/>
-      <c r="H40" s="37"/>
-      <c r="I40" s="38"/>
+      <c r="F40" s="35"/>
+      <c r="G40" s="36"/>
+      <c r="H40" s="35"/>
+      <c r="I40" s="36"/>
     </row>
     <row r="41" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F41" s="37"/>
-      <c r="G41" s="38"/>
-      <c r="H41" s="37"/>
-      <c r="I41" s="38"/>
+      <c r="F41" s="35"/>
+      <c r="G41" s="36"/>
+      <c r="H41" s="35"/>
+      <c r="I41" s="36"/>
     </row>
     <row r="42" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F42" s="37"/>
-      <c r="G42" s="38"/>
-      <c r="H42" s="37"/>
-      <c r="I42" s="38"/>
+      <c r="F42" s="35"/>
+      <c r="G42" s="36"/>
+      <c r="H42" s="35"/>
+      <c r="I42" s="36"/>
     </row>
     <row r="43" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F43" s="37"/>
-      <c r="G43" s="38"/>
-      <c r="H43" s="37"/>
-      <c r="I43" s="38"/>
+      <c r="F43" s="35"/>
+      <c r="G43" s="36"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="36"/>
     </row>
     <row r="44" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F44" s="37"/>
-      <c r="G44" s="38"/>
-      <c r="H44" s="37"/>
-      <c r="I44" s="38"/>
+      <c r="F44" s="35"/>
+      <c r="G44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="36"/>
     </row>
     <row r="45" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F45" s="37"/>
-      <c r="G45" s="38"/>
-      <c r="H45" s="37"/>
-      <c r="I45" s="38"/>
+      <c r="F45" s="35"/>
+      <c r="G45" s="36"/>
+      <c r="H45" s="35"/>
+      <c r="I45" s="36"/>
     </row>
     <row r="46" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F46" s="37"/>
-      <c r="G46" s="38"/>
-      <c r="H46" s="37"/>
-      <c r="I46" s="38"/>
+      <c r="F46" s="35"/>
+      <c r="G46" s="36"/>
+      <c r="H46" s="35"/>
+      <c r="I46" s="36"/>
     </row>
     <row r="47" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F47" s="37"/>
-      <c r="G47" s="38"/>
-      <c r="H47" s="37"/>
-      <c r="I47" s="38"/>
+      <c r="F47" s="35"/>
+      <c r="G47" s="36"/>
+      <c r="H47" s="35"/>
+      <c r="I47" s="36"/>
     </row>
     <row r="48" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F48" s="37"/>
-      <c r="G48" s="38"/>
-      <c r="H48" s="37"/>
-      <c r="I48" s="38"/>
+      <c r="F48" s="35"/>
+      <c r="G48" s="36"/>
+      <c r="H48" s="35"/>
+      <c r="I48" s="36"/>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="F49" s="37"/>
-      <c r="G49" s="38"/>
-      <c r="H49" s="37"/>
-      <c r="I49" s="38"/>
+      <c r="F49" s="35"/>
+      <c r="G49" s="36"/>
+      <c r="H49" s="35"/>
+      <c r="I49" s="36"/>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="F50" s="37"/>
-      <c r="G50" s="38"/>
-      <c r="H50" s="37"/>
-      <c r="I50" s="38"/>
+      <c r="F50" s="35"/>
+      <c r="G50" s="36"/>
+      <c r="H50" s="35"/>
+      <c r="I50" s="36"/>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="F51" s="37"/>
-      <c r="G51" s="38"/>
-      <c r="H51" s="37"/>
-      <c r="I51" s="38"/>
+      <c r="F51" s="35"/>
+      <c r="G51" s="36"/>
+      <c r="H51" s="35"/>
+      <c r="I51" s="36"/>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="F52" s="37"/>
-      <c r="G52" s="38"/>
-      <c r="H52" s="37"/>
-      <c r="I52" s="38"/>
+      <c r="F52" s="35"/>
+      <c r="G52" s="36"/>
+      <c r="H52" s="35"/>
+      <c r="I52" s="36"/>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="F53" s="37"/>
-      <c r="G53" s="38"/>
-      <c r="H53" s="37"/>
-      <c r="I53" s="38"/>
+      <c r="F53" s="35"/>
+      <c r="G53" s="36"/>
+      <c r="H53" s="35"/>
+      <c r="I53" s="36"/>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="F54" s="37"/>
-      <c r="G54" s="38"/>
-      <c r="H54" s="37"/>
-      <c r="I54" s="38"/>
+      <c r="F54" s="35"/>
+      <c r="G54" s="36"/>
+      <c r="H54" s="35"/>
+      <c r="I54" s="36"/>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="F55" s="37"/>
-      <c r="G55" s="38"/>
-      <c r="H55" s="37"/>
-      <c r="I55" s="38"/>
+      <c r="F55" s="35"/>
+      <c r="G55" s="36"/>
+      <c r="H55" s="35"/>
+      <c r="I55" s="36"/>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B58" s="39" t="s">
+      <c r="B58" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="C58" s="39" t="s">
+      <c r="C58" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="D58" s="39" t="s">
+      <c r="D58" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="E58" s="40" t="s">
+      <c r="E58" s="38" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B59" s="41" t="s">
+      <c r="B59" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="C59" s="41">
+      <c r="C59" s="39">
         <v>1</v>
       </c>
-      <c r="D59" s="41" t="s">
+      <c r="D59" s="39" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1626,121 +1623,121 @@
       <c r="E60" s="65"/>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B61" s="42"/>
-      <c r="C61" s="17" t="s">
+      <c r="B61" s="40"/>
+      <c r="C61" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D61" s="17" t="s">
+      <c r="D61" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E61" s="17" t="s">
+      <c r="E61" s="16" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B62" s="43" t="s">
+      <c r="B62" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="C62" s="44" t="s">
+      <c r="C62" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="D62" s="44"/>
-      <c r="E62" s="44" t="s">
-        <v>55</v>
+      <c r="D62" s="42"/>
+      <c r="E62" s="42" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B63" s="43" t="s">
+      <c r="B63" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="C63" s="44"/>
-      <c r="D63" s="44"/>
-      <c r="E63" s="44"/>
+      <c r="C63" s="42"/>
+      <c r="D63" s="42"/>
+      <c r="E63" s="42"/>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B64" s="43" t="s">
+      <c r="B64" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="C64" s="44" t="s">
+      <c r="C64" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="D64" s="44"/>
-      <c r="E64" s="44"/>
+      <c r="D64" s="42"/>
+      <c r="E64" s="42"/>
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B65" s="43" t="s">
+      <c r="B65" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="C65" s="44" t="s">
+      <c r="C65" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="D65" s="44"/>
-      <c r="E65" s="44"/>
+      <c r="D65" s="42"/>
+      <c r="E65" s="42"/>
     </row>
     <row r="66" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B66" s="43" t="s">
+      <c r="B66" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="C66" s="44" t="s">
+      <c r="C66" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="D66" s="44"/>
-      <c r="E66" s="44"/>
+      <c r="D66" s="42"/>
+      <c r="E66" s="42"/>
     </row>
     <row r="67" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B67" s="45" t="s">
+      <c r="B67" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="C67" s="46"/>
-      <c r="D67" s="44" t="s">
+      <c r="C67" s="44"/>
+      <c r="D67" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="E67" s="44" t="s">
-        <v>37</v>
+      <c r="E67" s="42" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="68" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B68" s="45" t="s">
+      <c r="B68" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="C68" s="46"/>
-      <c r="D68" s="44"/>
-      <c r="E68" s="44"/>
+      <c r="C68" s="44"/>
+      <c r="D68" s="42"/>
+      <c r="E68" s="42"/>
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B69" s="62" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C69" s="62"/>
       <c r="D69" s="62"/>
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B70" s="17" t="s">
+      <c r="B70" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C70" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="D70" s="17" t="s">
+      <c r="C70" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D70" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E70" s="17" t="s">
+      <c r="E70" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="F70" s="17" t="s">
+      <c r="F70" s="16" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B71" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="C71" s="44" t="s">
+      <c r="B71" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="C71" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="D71" s="44"/>
-      <c r="E71" s="44"/>
-      <c r="F71" s="44" t="s">
+      <c r="D71" s="42"/>
+      <c r="E71" s="42"/>
+      <c r="F71" s="42" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1752,72 +1749,72 @@
       <c r="D72" s="62"/>
     </row>
     <row r="73" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B73" s="17" t="s">
+      <c r="B73" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C73" s="17" t="s">
+      <c r="C73" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D73" s="17" t="s">
+      <c r="D73" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E73" s="17" t="s">
+      <c r="E73" s="16" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="74" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B74" s="44" t="s">
+      <c r="B74" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="C74" s="44" t="s">
-        <v>38</v>
-      </c>
-      <c r="D74" s="44"/>
-      <c r="E74" s="47"/>
+      <c r="C74" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="D74" s="42"/>
+      <c r="E74" s="45"/>
     </row>
     <row r="75" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B75" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="C75" s="44" t="s">
+      <c r="B75" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="C75" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="D75" s="44"/>
-      <c r="E75" s="47"/>
+      <c r="D75" s="42"/>
+      <c r="E75" s="45"/>
     </row>
     <row r="76" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B76" s="43" t="s">
+      <c r="B76" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="C76" s="44">
+      <c r="C76" s="42">
         <v>1</v>
       </c>
     </row>
     <row r="77" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B77" s="43" t="s">
+      <c r="B77" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="C77" s="44">
+      <c r="C77" s="42">
         <v>1</v>
       </c>
     </row>
     <row r="80" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B80" s="39" t="s">
+      <c r="B80" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="C80" s="39" t="s">
+      <c r="C80" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="D80" s="40"/>
-      <c r="E80" s="40" t="s">
-        <v>47</v>
+      <c r="D80" s="38"/>
+      <c r="E80" s="38" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="81" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B81" s="41" t="s">
+      <c r="B81" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="C81" s="41">
+      <c r="C81" s="39">
         <v>2</v>
       </c>
     </row>
@@ -1830,141 +1827,141 @@
       <c r="E82" s="65"/>
     </row>
     <row r="83" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B83" s="42"/>
-      <c r="C83" s="17" t="s">
+      <c r="B83" s="40"/>
+      <c r="C83" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D83" s="17" t="s">
+      <c r="D83" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E83" s="17" t="s">
+      <c r="E83" s="16" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="84" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B84" s="43" t="s">
+      <c r="B84" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="C84" s="48" t="s">
+      <c r="C84" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="D84" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="E84" s="48" t="s">
-        <v>51</v>
+      <c r="D84" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="E84" s="46" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="85" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B85" s="43" t="s">
+      <c r="B85" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="C85" s="48"/>
-      <c r="D85" s="48"/>
-      <c r="E85" s="48"/>
+      <c r="C85" s="46"/>
+      <c r="D85" s="46"/>
+      <c r="E85" s="46"/>
     </row>
     <row r="86" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B86" s="43" t="s">
+      <c r="B86" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="C86" s="48"/>
-      <c r="D86" s="48" t="s">
+      <c r="C86" s="46"/>
+      <c r="D86" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="E86" s="48"/>
+      <c r="E86" s="46"/>
     </row>
     <row r="87" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B87" s="43" t="s">
+      <c r="B87" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="C87" s="48"/>
-      <c r="D87" s="48" t="s">
+      <c r="C87" s="46"/>
+      <c r="D87" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="E87" s="48"/>
-      <c r="G87" s="49"/>
+      <c r="E87" s="46"/>
+      <c r="G87" s="47"/>
     </row>
     <row r="88" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B88" s="43" t="s">
+      <c r="B88" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="C88" s="48" t="s">
+      <c r="C88" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="D88" s="48"/>
-      <c r="E88" s="48"/>
+      <c r="D88" s="46"/>
+      <c r="E88" s="46"/>
     </row>
     <row r="89" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B89" s="43" t="s">
+      <c r="B89" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="C89" s="50"/>
-      <c r="D89" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="E89" s="48" t="s">
-        <v>51</v>
+      <c r="C89" s="48"/>
+      <c r="D89" s="46" t="s">
+        <v>32</v>
+      </c>
+      <c r="E89" s="46" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="90" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B90" s="43" t="s">
+      <c r="B90" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="C90" s="50"/>
-      <c r="D90" s="48"/>
-      <c r="E90" s="48"/>
+      <c r="C90" s="48"/>
+      <c r="D90" s="46"/>
+      <c r="E90" s="46"/>
     </row>
     <row r="91" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B91" s="62" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C91" s="62"/>
       <c r="D91" s="62"/>
-      <c r="H91" s="51"/>
-      <c r="I91" s="52"/>
-      <c r="J91" s="52"/>
+      <c r="H91" s="49"/>
+      <c r="I91" s="50"/>
+      <c r="J91" s="50"/>
     </row>
     <row r="92" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B92" s="17" t="s">
+      <c r="B92" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C92" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="D92" s="17" t="s">
+      <c r="C92" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D92" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E92" s="17" t="s">
+      <c r="E92" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="F92" s="17" t="s">
+      <c r="F92" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="H92" s="51"/>
-      <c r="I92" s="51"/>
-      <c r="J92" s="51"/>
-      <c r="K92" s="52"/>
-      <c r="L92" s="53"/>
-      <c r="M92" s="53"/>
-      <c r="N92" s="54"/>
+      <c r="H92" s="49"/>
+      <c r="I92" s="49"/>
+      <c r="J92" s="49"/>
+      <c r="K92" s="50"/>
+      <c r="L92" s="51"/>
+      <c r="M92" s="51"/>
+      <c r="N92" s="52"/>
     </row>
     <row r="93" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B93" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="C93" s="48" t="s">
+      <c r="B93" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="C93" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="D93" s="48"/>
-      <c r="E93" s="48"/>
-      <c r="F93" s="48" t="s">
+      <c r="D93" s="46"/>
+      <c r="E93" s="46"/>
+      <c r="F93" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="K93" s="51"/>
-      <c r="L93" s="53"/>
-      <c r="M93" s="53"/>
-      <c r="N93" s="53"/>
-      <c r="O93" s="55"/>
+      <c r="K93" s="49"/>
+      <c r="L93" s="51"/>
+      <c r="M93" s="51"/>
+      <c r="N93" s="51"/>
+      <c r="O93" s="53"/>
     </row>
     <row r="94" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B94" s="62" t="s">
@@ -1974,72 +1971,72 @@
       <c r="D94" s="62"/>
     </row>
     <row r="95" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B95" s="17" t="s">
+      <c r="B95" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C95" s="17" t="s">
+      <c r="C95" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D95" s="17" t="s">
+      <c r="D95" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E95" s="17" t="s">
+      <c r="E95" s="16" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="96" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B96" s="48" t="s">
+      <c r="B96" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="C96" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="D96" s="48"/>
-      <c r="E96" s="56"/>
+      <c r="C96" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="D96" s="46"/>
+      <c r="E96" s="54"/>
     </row>
     <row r="97" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B97" s="48" t="s">
-        <v>42</v>
-      </c>
-      <c r="C97" s="48" t="s">
+      <c r="B97" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="C97" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="D97" s="48"/>
-      <c r="E97" s="56"/>
+      <c r="D97" s="46"/>
+      <c r="E97" s="54"/>
     </row>
     <row r="98" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B98" s="43" t="s">
+      <c r="B98" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="C98" s="48">
+      <c r="C98" s="46">
         <v>2</v>
       </c>
     </row>
     <row r="99" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B99" s="43" t="s">
+      <c r="B99" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="C99" s="48">
+      <c r="C99" s="46">
         <v>1</v>
       </c>
     </row>
     <row r="102" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B102" s="39" t="s">
+      <c r="B102" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="C102" s="39" t="s">
+      <c r="C102" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="D102" s="40"/>
-      <c r="E102" s="40" t="s">
-        <v>48</v>
+      <c r="D102" s="38"/>
+      <c r="E102" s="38" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="103" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B103" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="C103" s="41">
+      <c r="B103" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="C103" s="39">
         <v>1</v>
       </c>
     </row>
@@ -2052,117 +2049,117 @@
       <c r="E104" s="65"/>
     </row>
     <row r="105" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B105" s="42"/>
-      <c r="C105" s="17" t="s">
+      <c r="B105" s="40"/>
+      <c r="C105" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D105" s="17" t="s">
+      <c r="D105" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E105" s="17" t="s">
+      <c r="E105" s="16" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="106" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B106" s="43" t="s">
+      <c r="B106" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="C106" s="57"/>
-      <c r="D106" s="57" t="s">
+      <c r="C106" s="55"/>
+      <c r="D106" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="E106" s="57" t="s">
+      <c r="E106" s="55" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="107" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B107" s="43" t="s">
+      <c r="B107" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="C107" s="57"/>
-      <c r="D107" s="57"/>
-      <c r="E107" s="57"/>
+      <c r="C107" s="55"/>
+      <c r="D107" s="55"/>
+      <c r="E107" s="55"/>
     </row>
     <row r="108" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B108" s="43" t="s">
+      <c r="B108" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="C108" s="57"/>
-      <c r="D108" s="57" t="s">
+      <c r="C108" s="55"/>
+      <c r="D108" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="E108" s="55"/>
+    </row>
+    <row r="109" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B109" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="C109" s="55"/>
+      <c r="D109" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="E108" s="57"/>
-    </row>
-    <row r="109" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B109" s="43" t="s">
-        <v>17</v>
-      </c>
-      <c r="C109" s="57"/>
-      <c r="D109" s="57" t="s">
-        <v>53</v>
-      </c>
-      <c r="E109" s="57"/>
+      <c r="E109" s="55"/>
     </row>
     <row r="110" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B110" s="43" t="s">
+      <c r="B110" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="C110" s="57" t="s">
+      <c r="C110" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="D110" s="57"/>
-      <c r="E110" s="57"/>
+      <c r="D110" s="55"/>
+      <c r="E110" s="55"/>
     </row>
     <row r="111" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B111" s="43" t="s">
+      <c r="B111" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="C111" s="50"/>
-      <c r="D111" s="57"/>
-      <c r="E111" s="57"/>
+      <c r="C111" s="48"/>
+      <c r="D111" s="55"/>
+      <c r="E111" s="55"/>
     </row>
     <row r="112" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B112" s="43" t="s">
+      <c r="B112" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="C112" s="50"/>
-      <c r="D112" s="57"/>
-      <c r="E112" s="57"/>
+      <c r="C112" s="48"/>
+      <c r="D112" s="55"/>
+      <c r="E112" s="55"/>
     </row>
     <row r="113" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B113" s="62" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C113" s="62"/>
       <c r="D113" s="62"/>
     </row>
     <row r="114" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B114" s="17" t="s">
+      <c r="B114" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C114" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="D114" s="17" t="s">
+      <c r="C114" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D114" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E114" s="17" t="s">
+      <c r="E114" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="F114" s="17" t="s">
+      <c r="F114" s="16" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="115" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B115" s="57" t="s">
-        <v>54</v>
-      </c>
-      <c r="C115" s="57" t="s">
+      <c r="B115" s="55" t="s">
+        <v>53</v>
+      </c>
+      <c r="C115" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="D115" s="57"/>
-      <c r="E115" s="57"/>
-      <c r="F115" s="57" t="s">
+      <c r="D115" s="55"/>
+      <c r="E115" s="55"/>
+      <c r="F115" s="55" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2174,72 +2171,72 @@
       <c r="D116" s="62"/>
     </row>
     <row r="117" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B117" s="17" t="s">
+      <c r="B117" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C117" s="17" t="s">
+      <c r="C117" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D117" s="17" t="s">
+      <c r="D117" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E117" s="17" t="s">
+      <c r="E117" s="16" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="118" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B118" s="57" t="s">
+      <c r="B118" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="C118" s="57" t="s">
+      <c r="C118" s="55" t="s">
+        <v>37</v>
+      </c>
+      <c r="D118" s="55"/>
+      <c r="E118" s="56"/>
+    </row>
+    <row r="119" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B119" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="C119" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="D119" s="55"/>
+      <c r="E119" s="56"/>
+    </row>
+    <row r="120" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B120" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C120" s="55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="121" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B121" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="C121" s="55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B124" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="C124" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D124" s="38"/>
+      <c r="E124" s="38" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="125" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B125" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="D118" s="57"/>
-      <c r="E118" s="58"/>
-    </row>
-    <row r="119" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B119" s="57" t="s">
-        <v>42</v>
-      </c>
-      <c r="C119" s="57" t="s">
-        <v>35</v>
-      </c>
-      <c r="D119" s="57"/>
-      <c r="E119" s="58"/>
-    </row>
-    <row r="120" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B120" s="43" t="s">
-        <v>24</v>
-      </c>
-      <c r="C120" s="57">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="121" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B121" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="C121" s="57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="124" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B124" s="39" t="s">
-        <v>6</v>
-      </c>
-      <c r="C124" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="D124" s="40"/>
-      <c r="E124" s="40" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="125" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B125" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="C125" s="41">
+      <c r="C125" s="39">
         <v>2</v>
       </c>
     </row>
@@ -2252,125 +2249,125 @@
       <c r="E126" s="65"/>
     </row>
     <row r="127" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B127" s="42"/>
-      <c r="C127" s="17" t="s">
+      <c r="B127" s="40"/>
+      <c r="C127" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D127" s="17" t="s">
+      <c r="D127" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E127" s="17" t="s">
+      <c r="E127" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="F127" s="17" t="s">
-        <v>56</v>
+      <c r="F127" s="16" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="128" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B128" s="43" t="s">
+      <c r="B128" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="C128" s="59" t="s">
+      <c r="C128" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="D128" s="59" t="s">
+      <c r="D128" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="E128" s="59" t="s">
-        <v>51</v>
+      <c r="E128" s="57" t="s">
+        <v>50</v>
       </c>
       <c r="F128" s="60" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="129" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B129" s="43" t="s">
+      <c r="B129" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="C129" s="59"/>
-      <c r="D129" s="59"/>
-      <c r="E129" s="59"/>
+      <c r="C129" s="57"/>
+      <c r="D129" s="57"/>
+      <c r="E129" s="57"/>
     </row>
     <row r="130" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B130" s="43" t="s">
+      <c r="B130" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="C130" s="59"/>
-      <c r="D130" s="59" t="s">
+      <c r="C130" s="57"/>
+      <c r="D130" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="E130" s="59"/>
+      <c r="E130" s="57"/>
     </row>
     <row r="131" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B131" s="43" t="s">
+      <c r="B131" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="C131" s="59"/>
-      <c r="D131" s="59" t="s">
+      <c r="C131" s="57"/>
+      <c r="D131" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="E131" s="59"/>
+      <c r="E131" s="57"/>
     </row>
     <row r="132" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B132" s="43" t="s">
+      <c r="B132" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="C132" s="59" t="s">
+      <c r="C132" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="D132" s="59"/>
-      <c r="E132" s="59"/>
+      <c r="D132" s="57"/>
+      <c r="E132" s="57"/>
     </row>
     <row r="133" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B133" s="43" t="s">
+      <c r="B133" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="C133" s="50"/>
-      <c r="D133" s="59"/>
-      <c r="E133" s="59"/>
+      <c r="C133" s="48"/>
+      <c r="D133" s="57"/>
+      <c r="E133" s="57"/>
     </row>
     <row r="134" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B134" s="43" t="s">
+      <c r="B134" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="C134" s="50"/>
-      <c r="D134" s="59"/>
-      <c r="E134" s="59"/>
+      <c r="C134" s="48"/>
+      <c r="D134" s="57"/>
+      <c r="E134" s="57"/>
     </row>
     <row r="135" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B135" s="62" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C135" s="62"/>
       <c r="D135" s="62"/>
     </row>
     <row r="136" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B136" s="17" t="s">
+      <c r="B136" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C136" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="D136" s="17" t="s">
+      <c r="C136" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D136" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E136" s="17" t="s">
+      <c r="E136" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="F136" s="17" t="s">
+      <c r="F136" s="16" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="137" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B137" s="59" t="s">
-        <v>54</v>
-      </c>
-      <c r="C137" s="59" t="s">
+      <c r="B137" s="57" t="s">
+        <v>53</v>
+      </c>
+      <c r="C137" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="D137" s="59"/>
-      <c r="E137" s="59"/>
-      <c r="F137" s="59" t="s">
+      <c r="D137" s="57"/>
+      <c r="E137" s="57"/>
+      <c r="F137" s="57" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2382,64 +2379,58 @@
       <c r="D138" s="65"/>
     </row>
     <row r="139" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B139" s="17" t="s">
+      <c r="B139" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C139" s="17" t="s">
+      <c r="C139" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D139" s="17" t="s">
+      <c r="D139" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E139" s="17" t="s">
+      <c r="E139" s="16" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="140" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B140" s="59" t="s">
+      <c r="B140" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="C140" s="59" t="s">
+      <c r="C140" s="57" t="s">
+        <v>38</v>
+      </c>
+      <c r="D140" s="57"/>
+      <c r="E140" s="58"/>
+    </row>
+    <row r="141" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B141" s="57" t="s">
+        <v>41</v>
+      </c>
+      <c r="C141" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="D140" s="59"/>
-      <c r="E140" s="61"/>
-    </row>
-    <row r="141" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B141" s="59" t="s">
-        <v>42</v>
-      </c>
-      <c r="C141" s="59" t="s">
-        <v>40</v>
-      </c>
-      <c r="D141" s="59"/>
-      <c r="E141" s="61"/>
+      <c r="D141" s="57"/>
+      <c r="E141" s="58"/>
     </row>
     <row r="142" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B142" s="43" t="s">
+      <c r="B142" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="C142" s="59">
+      <c r="C142" s="57">
         <v>4</v>
       </c>
     </row>
     <row r="143" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B143" s="43" t="s">
+      <c r="B143" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="C143" s="59">
+      <c r="C143" s="57">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="15">
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="B60:E60"/>
-    <mergeCell ref="B82:E82"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="F9:J9"/>
-    <mergeCell ref="B72:D72"/>
     <mergeCell ref="B116:D116"/>
     <mergeCell ref="B126:E126"/>
     <mergeCell ref="C9:D9"/>
@@ -2449,10 +2440,16 @@
     <mergeCell ref="B113:D113"/>
     <mergeCell ref="B135:D135"/>
     <mergeCell ref="B104:E104"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="B60:E60"/>
+    <mergeCell ref="B82:E82"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="F9:J9"/>
+    <mergeCell ref="B72:D72"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="92" orientation="landscape" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup scale="92" orientation="landscape" useFirstPageNumber="1" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;C&amp;F</oddHeader>
     <oddFooter>&amp;CPrepared by Claire Cook &amp;D&amp;RPage &amp;P</oddFooter>
@@ -2550,7 +2547,7 @@
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D67&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E67&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;after-invalid interval="8 weeks" grace="4 weeks 4 days"/&gt;</v>
+        <v xml:space="preserve">    &lt;after-invalid interval="8 weeks" grace="4 weeks"/&gt;</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
@@ -2628,7 +2625,7 @@
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D89&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E89&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;after-invalid interval="4 weeks" grace="4 days"/&gt;</v>
+        <v xml:space="preserve">    &lt;after-invalid interval="8 weeks" grace="4 weeks"/&gt;</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
@@ -2752,7 +2749,7 @@
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" s="12" t="str">
+      <c r="A46" s="61" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C128&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D128&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E128&amp;CHAR(34)&amp;" intervalGrace="&amp;CHAR(34)&amp;Schedules!F128&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="50 years" interval="8 weeks" grace="4 days" intervalGrace="8 weeks"/&gt;</v>
       </c>

</xml_diff>

<commit_message>
Zoster schedule update (2018-07-12)
</commit_message>
<xml_diff>
--- a/schedules/Zoster.xlsx
+++ b/schedules/Zoster.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TCHWorkspaceJava6\fv\schedules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Forecaster Schedule Updates\Zostre Updates\Zoster 2018-07-12\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4860" yWindow="0" windowWidth="16140" windowHeight="11025" tabRatio="283"/>
+    <workbookView xWindow="3555" yWindow="0" windowWidth="16140" windowHeight="11025" tabRatio="283"/>
   </bookViews>
   <sheets>
     <sheet name="Schedules" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="56">
   <si>
     <t>Forecast Series Name</t>
   </si>
@@ -740,9 +740,9 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
     <mruColors>
+      <color rgb="FFFFCCCC"/>
       <color rgb="FFCCFFCC"/>
       <color rgb="FFFFCCFF"/>
-      <color rgb="FFFFCCCC"/>
       <color rgb="FFCCCCFF"/>
       <color rgb="FF993300"/>
       <color rgb="FFFFFFCC"/>
@@ -766,19 +766,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>10582</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>60942</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>135438</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>154428</xdr:rowOff>
+      <xdr:colOff>259772</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>39551</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -797,8 +797,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="105834" y="2180165"/>
-          <a:ext cx="9120687" cy="6176346"/>
+          <a:off x="112568" y="2139124"/>
+          <a:ext cx="9724159" cy="6559518"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2059,7 +2059,9 @@
       <c r="B106" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="C106" s="55"/>
+      <c r="C106" s="55" t="s">
+        <v>29</v>
+      </c>
       <c r="D106" s="55" t="s">
         <v>32</v>
       </c>
@@ -2666,7 +2668,7 @@
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C106&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D106&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E106&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;valid age="" interval="8 weeks" grace="8 weeks"/&gt;</v>
+        <v xml:space="preserve">    &lt;valid age="50 years" interval="8 weeks" grace="8 weeks"/&gt;</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Change name from Shingrix (RZV) to Zoster in schedule
</commit_message>
<xml_diff>
--- a/schedules/Zoster.xlsx
+++ b/schedules/Zoster.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3555" yWindow="0" windowWidth="16140" windowHeight="11025" tabRatio="283"/>
+    <workbookView xWindow="4860" yWindow="0" windowWidth="16140" windowHeight="11025" tabRatio="283"/>
   </bookViews>
   <sheets>
     <sheet name="Schedules" sheetId="1" r:id="rId1"/>
@@ -187,10 +187,10 @@
     <t>32 years 4 days</t>
   </si>
   <si>
-    <t>RZV (Shingrix)</t>
-  </si>
-  <si>
     <t>Grace for Interval</t>
+  </si>
+  <si>
+    <t>Zoster</t>
   </si>
 </sst>
 </file>
@@ -654,17 +654,17 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1190,7 +1190,7 @@
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F2" s="62" t="s">
         <v>1</v>
@@ -1280,17 +1280,17 @@
       <c r="B9" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="68">
+      <c r="C9" s="66">
         <v>178</v>
       </c>
-      <c r="D9" s="69"/>
-      <c r="F9" s="66" t="s">
+      <c r="D9" s="67"/>
+      <c r="F9" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="G9" s="67"/>
-      <c r="H9" s="67"/>
-      <c r="I9" s="67"/>
-      <c r="J9" s="67"/>
+      <c r="G9" s="69"/>
+      <c r="H9" s="69"/>
+      <c r="I9" s="69"/>
+      <c r="J9" s="69"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B10" s="29"/>
@@ -2257,7 +2257,7 @@
         <v>13</v>
       </c>
       <c r="F127" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="128" spans="2:6" x14ac:dyDescent="0.2">
@@ -2426,6 +2426,12 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="15">
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="B60:E60"/>
+    <mergeCell ref="B82:E82"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="F9:J9"/>
+    <mergeCell ref="B72:D72"/>
     <mergeCell ref="B116:D116"/>
     <mergeCell ref="B126:E126"/>
     <mergeCell ref="C9:D9"/>
@@ -2435,12 +2441,6 @@
     <mergeCell ref="B113:D113"/>
     <mergeCell ref="B135:D135"/>
     <mergeCell ref="B104:E104"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="B60:E60"/>
-    <mergeCell ref="B82:E82"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="F9:J9"/>
-    <mergeCell ref="B72:D72"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2476,7 +2476,7 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="str">
         <f>"&lt;forecast seriesName="&amp;CHAR(34)&amp;Schedules!D2&amp;CHAR(34)&amp;"&gt;"</f>
-        <v>&lt;forecast seriesName="RZV (Shingrix)"&gt;</v>
+        <v>&lt;forecast seriesName="Zoster"&gt;</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>